<commit_message>
rewrite of introduction and methods
</commit_message>
<xml_diff>
--- a/data/TablesZhangetal2017_09_02_EN.xlsx
+++ b/data/TablesZhangetal2017_09_02_EN.xlsx
@@ -1,27 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nanin\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rver4657\Dropbox (Sydney Uni)\Research\Forest_and_water\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A10C8E4D-3A32-431B-B697-147E953D308B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{745EB532-EE80-4FF1-AAB6-4E52113BBE64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="30" windowWidth="19180" windowHeight="10170" xr2:uid="{B1C3C98C-7119-441C-AC65-FC55BF675211}"/>
+    <workbookView xWindow="18980" yWindow="0" windowWidth="19420" windowHeight="11400" activeTab="1" xr2:uid="{B1C3C98C-7119-441C-AC65-FC55BF675211}"/>
   </bookViews>
   <sheets>
     <sheet name="Zhang et al. (2017) &gt;1000km2" sheetId="1" r:id="rId1"/>
     <sheet name="Zhang et al. (2017) &lt; 1000 km2" sheetId="2" r:id="rId2"/>
     <sheet name="NewData" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -2576,9 +2584,6 @@
     <t xml:space="preserve">1982 and 2007 </t>
   </si>
   <si>
-    <t>only in japanese, it is in Bosch and hawlett review but cannot id catchment</t>
-  </si>
-  <si>
     <t>d</t>
   </si>
   <si>
@@ -2622,6 +2627,9 @@
   </si>
   <si>
     <t>The tree felling is actually incremental in time, so not really a single observation. In addition, there are no clear individual coordinates for the subcatchments in Plynlimon. Approximate location from  https://www.ceh.ac.uk/our-science/projects/plynlimon-experimental-catchments</t>
+  </si>
+  <si>
+    <t>only in japanese, it is in Bosch and hewlett review but cannot id catchment</t>
   </si>
 </sst>
 </file>
@@ -2631,7 +2639,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2913,18 +2921,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
@@ -2963,6 +2959,18 @@
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3282,27 +3290,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29CA6CB8-28F4-480A-8011-F310B3E1710B}">
   <dimension ref="A1:T62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="47" zoomScaleNormal="47" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+    <sheetView zoomScale="47" zoomScaleNormal="47" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="10" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="10.199999999999999"/>
   <cols>
-    <col min="1" max="10" width="8.7265625" style="17"/>
-    <col min="11" max="11" width="17.81640625" style="17" customWidth="1"/>
-    <col min="12" max="12" width="11.36328125" style="23" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.36328125" style="23" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.26953125" style="18" customWidth="1"/>
-    <col min="15" max="15" width="7.1796875" style="18" customWidth="1"/>
-    <col min="16" max="16" width="7.453125" style="18" customWidth="1"/>
-    <col min="17" max="17" width="18.90625" style="18" customWidth="1"/>
-    <col min="18" max="18" width="18.90625" style="20" customWidth="1"/>
-    <col min="19" max="19" width="21.54296875" style="17" customWidth="1"/>
-    <col min="20" max="20" width="9.7265625" style="17" customWidth="1"/>
-    <col min="21" max="16384" width="8.7265625" style="17"/>
+    <col min="1" max="10" width="8.77734375" style="17"/>
+    <col min="11" max="11" width="17.77734375" style="17" customWidth="1"/>
+    <col min="12" max="12" width="11.33203125" style="23" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.33203125" style="23" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.21875" style="18" customWidth="1"/>
+    <col min="15" max="15" width="7.21875" style="18" customWidth="1"/>
+    <col min="16" max="16" width="7.44140625" style="18" customWidth="1"/>
+    <col min="17" max="17" width="18.88671875" style="18" customWidth="1"/>
+    <col min="18" max="18" width="18.88671875" style="20" customWidth="1"/>
+    <col min="19" max="19" width="21.5546875" style="17" customWidth="1"/>
+    <col min="20" max="20" width="9.77734375" style="17" customWidth="1"/>
+    <col min="21" max="16384" width="8.77734375" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="53" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" ht="52.95" customHeight="1">
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
@@ -3364,7 +3372,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" ht="51">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -3427,7 +3435,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" ht="20.399999999999999">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -3490,7 +3498,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" ht="28.95" customHeight="1">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -3553,7 +3561,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="101.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" ht="101.55" customHeight="1">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -3613,7 +3621,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" ht="28.95" customHeight="1">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -3676,7 +3684,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" ht="28.95" customHeight="1">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -3736,7 +3744,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" ht="28.95" customHeight="1">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -3796,7 +3804,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" ht="28.95" customHeight="1">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -3856,7 +3864,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" ht="28.95" customHeight="1">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -3919,7 +3927,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" ht="28.95" customHeight="1">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -3979,7 +3987,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" ht="28.95" customHeight="1">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -4039,7 +4047,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" ht="28.95" customHeight="1">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -4099,70 +4107,70 @@
         <v>650</v>
       </c>
     </row>
-    <row r="14" spans="1:20" s="41" customFormat="1" ht="67" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="39">
+    <row r="14" spans="1:20" s="37" customFormat="1" ht="67.05" customHeight="1">
+      <c r="A14" s="35">
         <v>13</v>
       </c>
-      <c r="B14" s="39" t="s">
+      <c r="B14" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="C14" s="39">
+      <c r="C14" s="35">
         <v>1304</v>
       </c>
-      <c r="D14" s="39">
+      <c r="D14" s="35">
         <v>433.1</v>
       </c>
-      <c r="E14" s="39" t="s">
+      <c r="E14" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="F14" s="39" t="s">
-        <v>14</v>
-      </c>
-      <c r="G14" s="39">
+      <c r="F14" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="G14" s="35">
         <v>19</v>
       </c>
-      <c r="H14" s="39">
+      <c r="H14" s="35">
         <v>-29</v>
       </c>
-      <c r="I14" s="39" t="s">
-        <v>15</v>
-      </c>
-      <c r="J14" s="39" t="s">
+      <c r="I14" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="J14" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="K14" s="39" t="s">
+      <c r="K14" s="35" t="s">
         <v>646</v>
       </c>
-      <c r="L14" s="40">
+      <c r="L14" s="36">
         <v>38</v>
       </c>
-      <c r="M14" s="40">
+      <c r="M14" s="36">
         <v>112</v>
       </c>
-      <c r="N14" s="41" t="s">
+      <c r="N14" s="37" t="s">
         <v>574</v>
       </c>
-      <c r="O14" s="41">
+      <c r="O14" s="37">
         <v>1959</v>
       </c>
-      <c r="P14" s="41">
+      <c r="P14" s="37">
         <v>2000</v>
       </c>
-      <c r="Q14" s="41">
+      <c r="Q14" s="37">
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
       <c r="R14" s="21" t="s">
         <v>619</v>
       </c>
-      <c r="S14" s="41" t="s">
+      <c r="S14" s="37" t="s">
         <v>620</v>
       </c>
-      <c r="T14" s="41" t="s">
+      <c r="T14" s="37" t="s">
         <v>651</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" ht="28.95" customHeight="1">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -4222,7 +4230,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" ht="58.5" customHeight="1">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -4282,7 +4290,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:20" ht="28.95" customHeight="1">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -4325,8 +4333,8 @@
       <c r="N17" s="18" t="s">
         <v>577</v>
       </c>
-      <c r="O17" s="43"/>
-      <c r="P17" s="43"/>
+      <c r="O17" s="39"/>
+      <c r="P17" s="39"/>
       <c r="Q17" s="18">
         <v>1</v>
       </c>
@@ -4336,11 +4344,11 @@
       <c r="S17" s="18" t="s">
         <v>578</v>
       </c>
-      <c r="T17" s="42" t="s">
+      <c r="T17" s="38" t="s">
         <v>653</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="69.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" ht="69.45" customHeight="1">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -4400,7 +4408,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" ht="28.95" customHeight="1">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -4460,7 +4468,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" ht="28.95" customHeight="1">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -4520,7 +4528,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="21" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" ht="28.95" customHeight="1">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -4580,7 +4588,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="22" spans="1:20" ht="217.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" ht="217.5" customHeight="1">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -4640,7 +4648,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="23" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" ht="28.95" customHeight="1">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -4703,7 +4711,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="24" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" ht="28.95" customHeight="1">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -4746,17 +4754,17 @@
       <c r="N24" s="18" t="s">
         <v>597</v>
       </c>
-      <c r="O24" s="43">
+      <c r="O24" s="39">
         <v>1995</v>
       </c>
-      <c r="P24" s="43">
+      <c r="P24" s="39">
         <v>1996</v>
       </c>
-      <c r="Q24" s="43">
+      <c r="Q24" s="39">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="R24" s="44" t="s">
+      <c r="R24" s="40" t="s">
         <v>660</v>
       </c>
       <c r="S24" s="18" t="s">
@@ -4766,7 +4774,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="25" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" ht="28.95" customHeight="1">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -4809,13 +4817,13 @@
       <c r="N25" s="18" t="s">
         <v>597</v>
       </c>
-      <c r="O25" s="43">
+      <c r="O25" s="39">
         <v>1996</v>
       </c>
-      <c r="P25" s="43">
+      <c r="P25" s="39">
         <v>1996</v>
       </c>
-      <c r="Q25" s="43">
+      <c r="Q25" s="39">
         <v>1</v>
       </c>
       <c r="R25" s="20" t="s">
@@ -4828,7 +4836,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="26" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" ht="28.95" customHeight="1">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -4891,7 +4899,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="27" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" ht="28.95" customHeight="1">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -4949,7 +4957,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="28" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" ht="28.95" customHeight="1">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -5009,7 +5017,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="29" spans="1:20" ht="29.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:20" ht="29.55" customHeight="1" thickBot="1">
       <c r="A29" s="4">
         <v>28</v>
       </c>
@@ -5067,7 +5075,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="30" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20" ht="28.95" customHeight="1">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -5127,7 +5135,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="31" spans="1:20" ht="58" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" ht="58.05" customHeight="1">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -5187,7 +5195,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="32" spans="1:20" ht="58" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" ht="58.05" customHeight="1">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -5247,7 +5255,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="33" spans="1:20" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20" ht="46.5" customHeight="1">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -5310,7 +5318,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="34" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:20" ht="28.95" customHeight="1">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -5370,7 +5378,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="35" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:20" ht="28.95" customHeight="1">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -5425,7 +5433,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="36" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:20" ht="28.95" customHeight="1">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -5480,7 +5488,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="37" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:20" ht="28.95" customHeight="1">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -5540,7 +5548,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="38" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:20" ht="19.95" customHeight="1">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -5583,16 +5591,16 @@
       <c r="N38" s="18" t="s">
         <v>577</v>
       </c>
-      <c r="O38" s="43"/>
-      <c r="P38" s="43"/>
-      <c r="Q38" s="43">
+      <c r="O38" s="39"/>
+      <c r="P38" s="39"/>
+      <c r="Q38" s="39">
         <v>1</v>
       </c>
-      <c r="R38" s="44">
+      <c r="R38" s="40">
         <v>2000</v>
       </c>
     </row>
-    <row r="39" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20" ht="28.95" customHeight="1">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -5635,7 +5643,7 @@
       <c r="N39" s="18" t="s">
         <v>574</v>
       </c>
-      <c r="O39" s="43">
+      <c r="O39" s="39">
         <v>1883</v>
       </c>
       <c r="P39" s="18">
@@ -5652,7 +5660,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="40" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:20" ht="28.95" customHeight="1">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -5709,7 +5717,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="41" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:20" ht="28.95" customHeight="1">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -5769,7 +5777,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="42" spans="1:20" ht="71.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:20" ht="71.55" customHeight="1">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -5829,7 +5837,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="43" spans="1:20" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:20" ht="75" customHeight="1">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -5889,7 +5897,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="44" spans="1:20" ht="45.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:20" ht="45.45" customHeight="1">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -5932,19 +5940,19 @@
       <c r="N44" s="18" t="s">
         <v>577</v>
       </c>
-      <c r="O44" s="43"/>
-      <c r="P44" s="43"/>
+      <c r="O44" s="39"/>
+      <c r="P44" s="39"/>
       <c r="Q44" s="18">
         <v>1</v>
       </c>
-      <c r="R44" s="44">
+      <c r="R44" s="40">
         <v>2000</v>
       </c>
       <c r="S44" s="18" t="s">
         <v>579</v>
       </c>
     </row>
-    <row r="45" spans="1:20" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:20" ht="49.95" customHeight="1">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -5987,19 +5995,19 @@
       <c r="N45" s="18" t="s">
         <v>577</v>
       </c>
-      <c r="O45" s="43"/>
-      <c r="P45" s="43"/>
+      <c r="O45" s="39"/>
+      <c r="P45" s="39"/>
       <c r="Q45" s="18">
         <v>1</v>
       </c>
-      <c r="R45" s="44">
+      <c r="R45" s="40">
         <v>2000</v>
       </c>
       <c r="S45" s="18" t="s">
         <v>580</v>
       </c>
     </row>
-    <row r="46" spans="1:20" ht="47.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:20" ht="47.55" customHeight="1">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -6042,19 +6050,19 @@
       <c r="N46" s="18" t="s">
         <v>577</v>
       </c>
-      <c r="O46" s="43"/>
-      <c r="P46" s="43"/>
+      <c r="O46" s="39"/>
+      <c r="P46" s="39"/>
       <c r="Q46" s="18">
         <v>1</v>
       </c>
-      <c r="R46" s="44">
+      <c r="R46" s="40">
         <v>1995</v>
       </c>
       <c r="T46" s="22" t="s">
         <v>676</v>
       </c>
     </row>
-    <row r="47" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:20" ht="28.95" customHeight="1">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -6117,7 +6125,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="48" spans="1:20" ht="58" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:20" ht="58.05" customHeight="1">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -6160,19 +6168,19 @@
       <c r="N48" s="18" t="s">
         <v>577</v>
       </c>
-      <c r="O48" s="43"/>
-      <c r="P48" s="43"/>
+      <c r="O48" s="39"/>
+      <c r="P48" s="39"/>
       <c r="Q48" s="18">
         <v>1</v>
       </c>
-      <c r="R48" s="44">
+      <c r="R48" s="40">
         <v>2000</v>
       </c>
       <c r="S48" s="18" t="s">
         <v>581</v>
       </c>
     </row>
-    <row r="49" spans="1:20" ht="87" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:20" ht="87" customHeight="1">
       <c r="A49" s="2">
         <v>48</v>
       </c>
@@ -6235,7 +6243,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="50" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:20" ht="28.95" customHeight="1">
       <c r="A50" s="2">
         <v>49</v>
       </c>
@@ -6295,7 +6303,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="51" spans="1:20" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:20" ht="43.5" customHeight="1">
       <c r="A51" s="2">
         <v>50</v>
       </c>
@@ -6358,7 +6366,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="52" spans="1:20" ht="116" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:20" ht="115.95" customHeight="1">
       <c r="A52" s="2">
         <v>51</v>
       </c>
@@ -6421,7 +6429,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="53" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:20" ht="30.6">
       <c r="A53" s="2">
         <v>52</v>
       </c>
@@ -6481,7 +6489,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="54" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:20" ht="28.95" customHeight="1">
       <c r="A54" s="2">
         <v>53</v>
       </c>
@@ -6536,7 +6544,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="55" spans="1:20" ht="69.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:20" ht="69.45" customHeight="1">
       <c r="A55" s="2">
         <v>54</v>
       </c>
@@ -6596,7 +6604,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="56" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:20" ht="28.95" customHeight="1">
       <c r="A56" s="2">
         <v>55</v>
       </c>
@@ -6656,7 +6664,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="57" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:20" ht="28.95" customHeight="1">
       <c r="A57" s="2">
         <v>56</v>
       </c>
@@ -6716,7 +6724,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="58" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:20" ht="28.95" customHeight="1">
       <c r="A58" s="2">
         <v>57</v>
       </c>
@@ -6774,7 +6782,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="59" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:20" ht="28.95" customHeight="1">
       <c r="A59" s="2">
         <v>58</v>
       </c>
@@ -6834,7 +6842,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="60" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:20" ht="19.95" customHeight="1">
       <c r="A60" s="2">
         <v>59</v>
       </c>
@@ -6877,16 +6885,16 @@
       <c r="N60" s="18" t="s">
         <v>577</v>
       </c>
-      <c r="O60" s="43"/>
-      <c r="P60" s="43"/>
+      <c r="O60" s="39"/>
+      <c r="P60" s="39"/>
       <c r="Q60" s="18">
         <v>1</v>
       </c>
-      <c r="R60" s="44">
+      <c r="R60" s="40">
         <v>2000</v>
       </c>
     </row>
-    <row r="61" spans="1:20" ht="44.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:20" ht="44.55" customHeight="1">
       <c r="A61" s="2">
         <v>60</v>
       </c>
@@ -6946,7 +6954,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="62" spans="1:20" ht="48.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:20" ht="48.45" customHeight="1" thickBot="1">
       <c r="A62" s="4">
         <v>61</v>
       </c>
@@ -7024,23 +7032,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C628113C-78B0-4B5D-8B46-887DA17257C6}">
   <dimension ref="A1:T253"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="22" zoomScaleNormal="22" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A161" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="K1" sqref="K1"/>
-      <selection pane="bottomLeft" activeCell="H194" sqref="H194"/>
+      <selection pane="bottomLeft" activeCell="V169" sqref="V169"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="18.81640625" customWidth="1"/>
-    <col min="4" max="10" width="8.7265625" customWidth="1"/>
-    <col min="11" max="11" width="14.6328125" customWidth="1"/>
+    <col min="2" max="2" width="18.77734375" customWidth="1"/>
+    <col min="4" max="10" width="8.77734375" customWidth="1"/>
+    <col min="11" max="11" width="14.6640625" customWidth="1"/>
     <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.1796875" customWidth="1"/>
-    <col min="15" max="15" width="16.26953125" customWidth="1"/>
+    <col min="14" max="14" width="14.21875" customWidth="1"/>
+    <col min="15" max="15" width="16.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="21.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:20" ht="21.45" customHeight="1" thickBot="1">
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
@@ -7099,7 +7107,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="30" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:20" ht="30.6">
       <c r="A2" s="6">
         <v>158</v>
       </c>
@@ -7145,7 +7153,7 @@
         <v>709</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:20">
       <c r="A3" s="2">
         <v>264</v>
       </c>
@@ -7200,7 +7208,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:20">
       <c r="A4" s="2">
         <v>265</v>
       </c>
@@ -7255,7 +7263,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:20">
       <c r="A5" s="2">
         <v>157</v>
       </c>
@@ -7310,7 +7318,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:20" ht="19.95" customHeight="1">
       <c r="A6" s="2">
         <v>153</v>
       </c>
@@ -7365,7 +7373,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:20">
       <c r="A7" s="2">
         <v>156</v>
       </c>
@@ -7420,7 +7428,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:20" ht="20.399999999999999">
       <c r="A8" s="2">
         <v>124</v>
       </c>
@@ -7472,7 +7480,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:20">
       <c r="A9" s="2">
         <v>76</v>
       </c>
@@ -7527,7 +7535,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:20">
       <c r="A10" s="2">
         <v>210</v>
       </c>
@@ -7579,7 +7587,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:20">
       <c r="A11" s="9">
         <v>90</v>
       </c>
@@ -7638,7 +7646,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:20">
       <c r="A12" s="2">
         <v>199</v>
       </c>
@@ -7697,7 +7705,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:20">
       <c r="A13" s="9">
         <v>256</v>
       </c>
@@ -7756,7 +7764,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:20">
       <c r="A14" s="2">
         <v>257</v>
       </c>
@@ -7815,7 +7823,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:20" ht="20.399999999999999">
       <c r="A15" s="2">
         <v>292</v>
       </c>
@@ -7869,7 +7877,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:20">
       <c r="A16" s="2">
         <v>73</v>
       </c>
@@ -7929,7 +7937,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:20">
       <c r="A17" s="2">
         <v>89</v>
       </c>
@@ -7989,7 +7997,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:20">
       <c r="A18" s="2">
         <v>97</v>
       </c>
@@ -8049,7 +8057,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:20">
       <c r="A19" s="2">
         <v>123</v>
       </c>
@@ -8109,7 +8117,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:20">
       <c r="A20" s="2">
         <v>132</v>
       </c>
@@ -8169,7 +8177,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:20">
       <c r="A21" s="2">
         <v>161</v>
       </c>
@@ -8229,7 +8237,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:20">
       <c r="A22" s="2">
         <v>162</v>
       </c>
@@ -8289,7 +8297,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:20">
       <c r="A23" s="2">
         <v>163</v>
       </c>
@@ -8349,7 +8357,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:20">
       <c r="A24" s="2">
         <v>181</v>
       </c>
@@ -8409,7 +8417,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:20">
       <c r="A25" s="2">
         <v>244</v>
       </c>
@@ -8469,7 +8477,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:20">
       <c r="A26" s="2">
         <v>271</v>
       </c>
@@ -8529,7 +8537,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:20">
       <c r="A27" s="2">
         <v>283</v>
       </c>
@@ -8589,7 +8597,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="28" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:20" ht="15" thickBot="1">
       <c r="A28" s="2">
         <v>129</v>
       </c>
@@ -8644,7 +8652,7 @@
       </c>
       <c r="S28" s="31"/>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:20">
       <c r="A29" s="2">
         <v>131</v>
       </c>
@@ -8697,7 +8705,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="30" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:20" ht="15" thickBot="1">
       <c r="A30" s="4">
         <v>224</v>
       </c>
@@ -8754,7 +8762,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:20">
       <c r="A31" s="2">
         <v>70</v>
       </c>
@@ -8808,7 +8816,7 @@
         <v>1989</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:20">
       <c r="A32" s="2">
         <v>71</v>
       </c>
@@ -8862,7 +8870,7 @@
         <v>1989</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:19">
       <c r="A33" s="2">
         <v>168</v>
       </c>
@@ -8916,7 +8924,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:19">
       <c r="A34" s="2">
         <v>169</v>
       </c>
@@ -8967,7 +8975,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:19">
       <c r="A35" s="2">
         <v>170</v>
       </c>
@@ -9021,7 +9029,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:19">
       <c r="A36" s="2">
         <v>171</v>
       </c>
@@ -9072,7 +9080,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:19">
       <c r="A37" s="2">
         <v>274</v>
       </c>
@@ -9117,7 +9125,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:19" ht="20.399999999999999">
       <c r="A38" s="2">
         <v>77</v>
       </c>
@@ -9174,7 +9182,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="39" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:19" ht="20.399999999999999">
       <c r="A39" s="2">
         <v>102</v>
       </c>
@@ -9225,7 +9233,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:19" ht="20.399999999999999">
       <c r="A40" s="2">
         <v>117</v>
       </c>
@@ -9282,7 +9290,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="41" spans="1:19" ht="15" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:19" ht="20.399999999999999">
       <c r="A41" s="2">
         <v>64</v>
       </c>
@@ -9332,7 +9340,7 @@
         <v>1974</v>
       </c>
     </row>
-    <row r="42" spans="1:19" ht="15" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:19" ht="20.399999999999999">
       <c r="A42" s="2">
         <v>65</v>
       </c>
@@ -9383,7 +9391,7 @@
         <v>1974</v>
       </c>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:19">
       <c r="A43" s="2">
         <v>251</v>
       </c>
@@ -9437,7 +9445,7 @@
         <v>1966</v>
       </c>
     </row>
-    <row r="44" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:19" ht="20.399999999999999">
       <c r="A44" s="2">
         <v>94</v>
       </c>
@@ -9494,7 +9502,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:19">
       <c r="A45" s="2">
         <v>105</v>
       </c>
@@ -9548,7 +9556,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:19">
       <c r="A46" s="2">
         <v>241</v>
       </c>
@@ -9600,7 +9608,7 @@
         <v>1996</v>
       </c>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:19">
       <c r="A47" s="2">
         <v>259</v>
       </c>
@@ -9636,7 +9644,7 @@
       </c>
       <c r="L47" s="27"/>
     </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:19">
       <c r="A48" s="2">
         <v>270</v>
       </c>
@@ -9686,7 +9694,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:19">
       <c r="A49" s="2">
         <v>278</v>
       </c>
@@ -9739,7 +9747,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:19">
       <c r="A50" s="2">
         <v>295</v>
       </c>
@@ -9789,7 +9797,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:19">
       <c r="A51" s="2">
         <v>74</v>
       </c>
@@ -9843,7 +9851,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="52" spans="1:19" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:19" ht="33" customHeight="1">
       <c r="A52" s="2">
         <v>68</v>
       </c>
@@ -9890,7 +9898,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="53" spans="1:19" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:19" ht="20.55" customHeight="1">
       <c r="A53" s="2">
         <v>69</v>
       </c>
@@ -9926,7 +9934,7 @@
       </c>
       <c r="L53" s="32"/>
     </row>
-    <row r="54" spans="1:19" ht="50" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:19" ht="51">
       <c r="A54" s="2">
         <v>128</v>
       </c>
@@ -9979,7 +9987,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:19">
       <c r="A55" s="2">
         <v>188</v>
       </c>
@@ -10017,7 +10025,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="56" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:19" ht="15" thickBot="1">
       <c r="A56" s="4">
         <v>189</v>
       </c>
@@ -10055,7 +10063,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:19">
       <c r="A57" s="2">
         <v>197</v>
       </c>
@@ -10093,7 +10101,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:19" ht="20.399999999999999">
       <c r="A58" s="9">
         <v>200</v>
       </c>
@@ -10131,7 +10139,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:19">
       <c r="A59" s="2">
         <v>252</v>
       </c>
@@ -10169,7 +10177,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:19">
       <c r="A60" s="2">
         <v>253</v>
       </c>
@@ -10207,7 +10215,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:19">
       <c r="A61" s="2">
         <v>254</v>
       </c>
@@ -10245,7 +10253,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:19">
       <c r="A62" s="2">
         <v>130</v>
       </c>
@@ -10302,7 +10310,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:19">
       <c r="A63" s="2">
         <v>150</v>
       </c>
@@ -10359,7 +10367,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:19">
       <c r="A64" s="2">
         <v>249</v>
       </c>
@@ -10413,7 +10421,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="65" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:19" ht="20.399999999999999">
       <c r="A65" s="2">
         <v>204</v>
       </c>
@@ -10470,7 +10478,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="66" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:19">
       <c r="A66" s="2">
         <v>216</v>
       </c>
@@ -10524,7 +10532,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="67" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:19" ht="20.399999999999999">
       <c r="A67" s="2">
         <v>285</v>
       </c>
@@ -10575,7 +10583,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="68" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:19">
       <c r="A68" s="2">
         <v>88</v>
       </c>
@@ -10633,7 +10641,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="69" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:19" ht="20.399999999999999">
       <c r="A69" s="2">
         <v>72</v>
       </c>
@@ -10686,7 +10694,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="70" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:19" ht="20.399999999999999">
       <c r="A70" s="2">
         <v>83</v>
       </c>
@@ -10739,7 +10747,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="71" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:19" ht="20.399999999999999">
       <c r="A71" s="2">
         <v>103</v>
       </c>
@@ -10792,7 +10800,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="72" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:19" ht="20.399999999999999">
       <c r="A72" s="2">
         <v>182</v>
       </c>
@@ -10845,7 +10853,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="73" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:19">
       <c r="A73" s="2">
         <v>191</v>
       </c>
@@ -10898,7 +10906,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="74" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:19">
       <c r="A74" s="2">
         <v>100</v>
       </c>
@@ -10951,7 +10959,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="75" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:19">
       <c r="A75" s="2">
         <v>84</v>
       </c>
@@ -11006,7 +11014,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="76" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:19">
       <c r="A76" s="2">
         <v>205</v>
       </c>
@@ -11061,7 +11069,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="77" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:19" ht="20.399999999999999">
       <c r="A77" s="2">
         <v>211</v>
       </c>
@@ -11104,7 +11112,7 @@
       <c r="R77" s="10"/>
       <c r="S77" s="10"/>
     </row>
-    <row r="78" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:19">
       <c r="A78" s="2">
         <v>80</v>
       </c>
@@ -11159,7 +11167,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="79" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:19">
       <c r="A79" s="2">
         <v>81</v>
       </c>
@@ -11214,7 +11222,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="80" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:19">
       <c r="A80" s="2">
         <v>82</v>
       </c>
@@ -11269,7 +11277,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="81" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:19">
       <c r="A81" s="2">
         <v>192</v>
       </c>
@@ -11324,7 +11332,7 @@
       </c>
       <c r="S81" s="31"/>
     </row>
-    <row r="82" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:19">
       <c r="A82" s="2">
         <v>231</v>
       </c>
@@ -11381,7 +11389,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="83" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:19" ht="20.399999999999999">
       <c r="A83" s="9">
         <v>287</v>
       </c>
@@ -11436,7 +11444,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="84" spans="1:19" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:19" ht="21" thickBot="1">
       <c r="A84" s="4">
         <v>288</v>
       </c>
@@ -11491,7 +11499,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="85" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:19" ht="20.399999999999999">
       <c r="A85" s="2">
         <v>289</v>
       </c>
@@ -11546,7 +11554,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="86" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:19" ht="20.399999999999999">
       <c r="A86" s="2">
         <v>290</v>
       </c>
@@ -11601,7 +11609,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="87" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:19">
       <c r="A87" s="2">
         <v>273</v>
       </c>
@@ -11649,7 +11657,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="88" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:19">
       <c r="A88" s="2">
         <v>66</v>
       </c>
@@ -11703,7 +11711,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="89" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:19">
       <c r="A89" s="2">
         <v>119</v>
       </c>
@@ -11757,11 +11765,11 @@
         <v>577</v>
       </c>
     </row>
-    <row r="90" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:19">
       <c r="A90" s="9">
         <v>172</v>
       </c>
-      <c r="B90" s="51" t="s">
+      <c r="B90" s="47" t="s">
         <v>303</v>
       </c>
       <c r="C90" s="9">
@@ -11808,7 +11816,7 @@
         <v>1973</v>
       </c>
     </row>
-    <row r="91" spans="1:19" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:19" ht="19.95" customHeight="1">
       <c r="A91" s="2">
         <v>173</v>
       </c>
@@ -11850,11 +11858,11 @@
         <v>765</v>
       </c>
     </row>
-    <row r="92" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:19">
       <c r="A92" s="2">
         <v>174</v>
       </c>
-      <c r="B92" s="50" t="s">
+      <c r="B92" s="46" t="s">
         <v>306</v>
       </c>
       <c r="C92" s="2">
@@ -11904,7 +11912,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="93" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:19" ht="20.399999999999999">
       <c r="A93" s="2">
         <v>175</v>
       </c>
@@ -11943,7 +11951,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="94" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:19" ht="20.399999999999999">
       <c r="A94" s="2">
         <v>176</v>
       </c>
@@ -11982,46 +11990,46 @@
         <v>770</v>
       </c>
     </row>
-    <row r="95" spans="1:19" ht="20" x14ac:dyDescent="0.35">
-      <c r="A95" s="56">
+    <row r="95" spans="1:19" ht="20.399999999999999">
+      <c r="A95" s="52">
         <v>237</v>
       </c>
-      <c r="B95" s="56" t="s">
+      <c r="B95" s="52" t="s">
         <v>409</v>
       </c>
-      <c r="C95" s="56">
+      <c r="C95" s="52">
         <v>4.9299999999999997E-2</v>
       </c>
-      <c r="D95" s="56">
+      <c r="D95" s="52">
         <v>1317</v>
       </c>
-      <c r="E95" s="56" t="s">
+      <c r="E95" s="52" t="s">
         <v>24</v>
       </c>
-      <c r="F95" s="56" t="s">
-        <v>14</v>
-      </c>
-      <c r="G95" s="56">
+      <c r="F95" s="52" t="s">
+        <v>14</v>
+      </c>
+      <c r="G95" s="52">
         <v>0</v>
       </c>
-      <c r="H95" s="56">
+      <c r="H95" s="52">
         <v>0</v>
       </c>
-      <c r="I95" s="56" t="s">
-        <v>15</v>
-      </c>
-      <c r="J95" s="56" t="s">
-        <v>16</v>
-      </c>
-      <c r="K95" s="56" t="s">
+      <c r="I95" s="52" t="s">
+        <v>15</v>
+      </c>
+      <c r="J95" s="52" t="s">
+        <v>16</v>
+      </c>
+      <c r="K95" s="52" t="s">
         <v>410</v>
       </c>
-      <c r="L95" s="56"/>
-      <c r="M95" s="56" t="s">
+      <c r="L95" s="52"/>
+      <c r="M95" s="52" t="s">
         <v>770</v>
       </c>
     </row>
-    <row r="96" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:19">
       <c r="A96" s="2">
         <v>154</v>
       </c>
@@ -12075,7 +12083,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="97" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:19" ht="20.399999999999999">
       <c r="A97" s="2">
         <v>233</v>
       </c>
@@ -12114,7 +12122,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="98" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:19" ht="20.399999999999999">
       <c r="A98" s="2">
         <v>235</v>
       </c>
@@ -12153,7 +12161,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="99" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:19" ht="20.399999999999999">
       <c r="A99" s="2">
         <v>234</v>
       </c>
@@ -12192,7 +12200,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="100" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:19">
       <c r="A100" s="2">
         <v>155</v>
       </c>
@@ -12250,7 +12258,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="101" spans="1:19" ht="23" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:19" ht="22.95" customHeight="1">
       <c r="A101" s="9">
         <v>62</v>
       </c>
@@ -12308,7 +12316,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="102" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:19" ht="20.399999999999999">
       <c r="A102" s="2">
         <v>63</v>
       </c>
@@ -12366,7 +12374,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="103" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:19" ht="20.399999999999999">
       <c r="A103" s="2">
         <v>255</v>
       </c>
@@ -12405,7 +12413,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="104" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:19">
       <c r="A104" s="2">
         <v>104</v>
       </c>
@@ -12463,7 +12471,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="105" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:19">
       <c r="A105" s="2">
         <v>122</v>
       </c>
@@ -12518,7 +12526,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="106" spans="1:19" ht="30" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:19" ht="30.6">
       <c r="A106" s="2">
         <v>112</v>
       </c>
@@ -12563,7 +12571,7 @@
         <f>R106-Q106</f>
         <v>2</v>
       </c>
-      <c r="P106" s="47" t="s">
+      <c r="P106" s="43" t="s">
         <v>773</v>
       </c>
       <c r="Q106" s="10">
@@ -12573,7 +12581,7 @@
         <v>1964</v>
       </c>
     </row>
-    <row r="107" spans="1:19" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:19" ht="39.450000000000003" customHeight="1">
       <c r="A107" s="2">
         <v>111</v>
       </c>
@@ -12631,7 +12639,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="108" spans="1:19" ht="22" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:19" ht="22.05" customHeight="1">
       <c r="A108" s="2">
         <v>164</v>
       </c>
@@ -12670,7 +12678,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="109" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:19" ht="20.399999999999999">
       <c r="A109" s="2">
         <v>304</v>
       </c>
@@ -12721,7 +12729,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="110" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:19" ht="20.399999999999999">
       <c r="A110" s="2">
         <v>305</v>
       </c>
@@ -12772,7 +12780,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="111" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:19" ht="20.399999999999999">
       <c r="A111" s="2">
         <v>303</v>
       </c>
@@ -12820,7 +12828,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="112" spans="1:19" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="112" spans="1:19" ht="31.2" thickBot="1">
       <c r="A112" s="4">
         <v>276</v>
       </c>
@@ -12868,7 +12876,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="113" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:19" ht="24" customHeight="1">
       <c r="A113" s="2">
         <v>221</v>
       </c>
@@ -12908,7 +12916,7 @@
       <c r="M113" s="10"/>
       <c r="N113" s="10"/>
     </row>
-    <row r="114" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:19" ht="30" customHeight="1">
       <c r="A114" s="2">
         <v>220</v>
       </c>
@@ -12959,7 +12967,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="115" spans="1:19" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:19" ht="28.5" customHeight="1">
       <c r="A115" s="2">
         <v>226</v>
       </c>
@@ -12998,7 +13006,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="116" spans="1:19" ht="30" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:19" ht="30.6">
       <c r="A116" s="2">
         <v>260</v>
       </c>
@@ -13049,7 +13057,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="117" spans="1:19" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:19" ht="31.5" customHeight="1">
       <c r="A117" s="2">
         <v>75</v>
       </c>
@@ -13099,7 +13107,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="118" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:19" ht="30.6">
       <c r="A118" s="2">
         <v>277</v>
       </c>
@@ -13149,7 +13157,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="119" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:19" ht="20.399999999999999">
       <c r="A119" s="2">
         <v>225</v>
       </c>
@@ -13193,14 +13201,14 @@
         <v>-111.548249</v>
       </c>
       <c r="O119" s="10"/>
-      <c r="P119" s="48" t="s">
+      <c r="P119" s="44" t="s">
         <v>781</v>
       </c>
       <c r="S119" t="s">
         <v>577</v>
       </c>
     </row>
-    <row r="120" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:19">
       <c r="A120" s="2">
         <v>307</v>
       </c>
@@ -13244,7 +13252,7 @@
       <c r="O120">
         <v>1</v>
       </c>
-      <c r="P120" s="48" t="s">
+      <c r="P120" s="44" t="s">
         <v>808</v>
       </c>
       <c r="Q120">
@@ -13257,7 +13265,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="121" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:19">
       <c r="A121" s="2">
         <v>308</v>
       </c>
@@ -13301,7 +13309,7 @@
       <c r="O121">
         <v>3</v>
       </c>
-      <c r="P121" s="48" t="s">
+      <c r="P121" s="44" t="s">
         <v>809</v>
       </c>
       <c r="Q121">
@@ -13314,7 +13322,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="122" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:19">
       <c r="A122" s="2">
         <v>309</v>
       </c>
@@ -13358,7 +13366,7 @@
       <c r="O122">
         <v>1</v>
       </c>
-      <c r="P122" s="48" t="s">
+      <c r="P122" s="44" t="s">
         <v>810</v>
       </c>
       <c r="Q122">
@@ -13371,7 +13379,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="123" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:19">
       <c r="A123" s="2">
         <v>310</v>
       </c>
@@ -13414,80 +13422,80 @@
         <f>-71-43/60-22.21/3600</f>
         <v>-71.722836111111107</v>
       </c>
-      <c r="O123" s="53">
+      <c r="O123" s="49">
         <v>4</v>
       </c>
-      <c r="P123" s="54" t="s">
+      <c r="P123" s="50" t="s">
         <v>807</v>
       </c>
-      <c r="Q123" s="53">
+      <c r="Q123" s="49">
         <v>1971</v>
       </c>
-      <c r="R123" s="53">
+      <c r="R123" s="49">
         <v>1974</v>
       </c>
-      <c r="S123" s="53" t="s">
+      <c r="S123" s="49" t="s">
         <v>577</v>
       </c>
     </row>
-    <row r="124" spans="1:19" s="53" customFormat="1" ht="20" x14ac:dyDescent="0.35">
-      <c r="A124" s="52">
+    <row r="124" spans="1:19" s="49" customFormat="1" ht="20.399999999999999">
+      <c r="A124" s="48">
         <v>179</v>
       </c>
-      <c r="B124" s="52" t="s">
+      <c r="B124" s="48" t="s">
         <v>312</v>
       </c>
-      <c r="C124" s="52">
+      <c r="C124" s="48">
         <v>0.16</v>
       </c>
-      <c r="D124" s="52">
+      <c r="D124" s="48">
         <v>1219</v>
       </c>
-      <c r="E124" s="52" t="s">
+      <c r="E124" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="F124" s="52" t="s">
-        <v>14</v>
-      </c>
-      <c r="G124" s="52">
+      <c r="F124" s="48" t="s">
+        <v>14</v>
+      </c>
+      <c r="G124" s="48">
         <v>-100</v>
       </c>
-      <c r="H124" s="52">
+      <c r="H124" s="48">
         <v>48.3</v>
       </c>
-      <c r="I124" s="52" t="s">
-        <v>15</v>
-      </c>
-      <c r="J124" s="52" t="s">
-        <v>16</v>
-      </c>
-      <c r="K124" s="52" t="s">
+      <c r="I124" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="J124" s="48" t="s">
+        <v>16</v>
+      </c>
+      <c r="K124" s="48" t="s">
         <v>313</v>
       </c>
-      <c r="L124" s="52"/>
+      <c r="L124" s="48"/>
       <c r="M124">
         <v>43.859166000000002</v>
       </c>
       <c r="N124">
         <v>-71.731251999999998</v>
       </c>
-      <c r="O124" s="53">
+      <c r="O124" s="49">
         <v>1</v>
       </c>
-      <c r="P124" s="54" t="s">
+      <c r="P124" s="50" t="s">
         <v>813</v>
       </c>
-      <c r="Q124" s="53">
+      <c r="Q124" s="49">
         <v>1966</v>
       </c>
-      <c r="R124" s="53">
+      <c r="R124" s="49">
         <v>1967</v>
       </c>
-      <c r="S124" s="53" t="s">
+      <c r="S124" s="49" t="s">
         <v>574</v>
       </c>
     </row>
-    <row r="125" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:19">
       <c r="A125" s="2">
         <v>209</v>
       </c>
@@ -13531,7 +13539,7 @@
       <c r="O125">
         <v>1</v>
       </c>
-      <c r="P125" s="48" t="s">
+      <c r="P125" s="44" t="s">
         <v>811</v>
       </c>
       <c r="Q125">
@@ -13544,7 +13552,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="126" spans="1:19" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:19" ht="28.95" customHeight="1">
       <c r="A126" s="2">
         <v>180</v>
       </c>
@@ -13588,14 +13596,14 @@
       <c r="O126" s="10" t="s">
         <v>814</v>
       </c>
-      <c r="P126" s="53" t="s">
+      <c r="P126" s="49" t="s">
         <v>812</v>
       </c>
       <c r="S126" t="s">
         <v>574</v>
       </c>
     </row>
-    <row r="127" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:19">
       <c r="A127" s="2">
         <v>190</v>
       </c>
@@ -13649,7 +13657,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="128" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:19">
       <c r="A128" s="2">
         <v>284</v>
       </c>
@@ -13703,7 +13711,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="129" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:19" ht="20.399999999999999">
       <c r="A129" s="2">
         <v>275</v>
       </c>
@@ -13751,7 +13759,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="130" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:19" ht="20.399999999999999">
       <c r="A130" s="2">
         <v>91</v>
       </c>
@@ -13806,7 +13814,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="131" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:19" ht="20.399999999999999">
       <c r="A131" s="2">
         <v>217</v>
       </c>
@@ -13861,7 +13869,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="132" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:19" ht="20.399999999999999">
       <c r="A132" s="2">
         <v>218</v>
       </c>
@@ -13916,7 +13924,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="133" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:19" ht="20.399999999999999">
       <c r="A133" s="2">
         <v>245</v>
       </c>
@@ -13971,63 +13979,63 @@
         <v>577</v>
       </c>
     </row>
-    <row r="134" spans="1:19" s="46" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A134" s="55"/>
-      <c r="B134" s="55" t="s">
+    <row r="134" spans="1:19" s="42" customFormat="1" ht="19.05" customHeight="1">
+      <c r="A134" s="51"/>
+      <c r="B134" s="51" t="s">
         <v>43</v>
       </c>
-      <c r="C134" s="55">
+      <c r="C134" s="51">
         <v>1545</v>
       </c>
-      <c r="D134" s="55">
+      <c r="D134" s="51">
         <v>1700</v>
       </c>
-      <c r="E134" s="55" t="s">
+      <c r="E134" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="F134" s="55" t="s">
-        <v>14</v>
-      </c>
-      <c r="G134" s="55">
+      <c r="F134" s="51" t="s">
+        <v>14</v>
+      </c>
+      <c r="G134" s="51">
         <v>15.19</v>
       </c>
-      <c r="H134" s="55">
+      <c r="H134" s="51">
         <v>-19.5</v>
       </c>
-      <c r="I134" s="55" t="s">
-        <v>15</v>
-      </c>
-      <c r="J134" s="55" t="s">
+      <c r="I134" s="51" t="s">
+        <v>15</v>
+      </c>
+      <c r="J134" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="K134" s="55" t="s">
+      <c r="K134" s="51" t="s">
         <v>44</v>
       </c>
-      <c r="L134" s="55"/>
-      <c r="M134" s="46">
+      <c r="L134" s="51"/>
+      <c r="M134" s="42">
         <v>-37.552613000000001</v>
       </c>
-      <c r="N134" s="46">
+      <c r="N134" s="42">
         <v>-72.010281000000006</v>
       </c>
       <c r="O134">
         <f t="shared" si="1"/>
         <v>43</v>
       </c>
-      <c r="P134" s="46" t="s">
+      <c r="P134" s="42" t="s">
         <v>815</v>
       </c>
-      <c r="Q134" s="46">
+      <c r="Q134" s="42">
         <v>1962</v>
       </c>
-      <c r="R134" s="46">
+      <c r="R134" s="42">
         <v>2005</v>
       </c>
       <c r="S134" t="s">
         <v>577</v>
       </c>
     </row>
-    <row r="135" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:19" ht="20.399999999999999">
       <c r="A135" s="2">
         <v>246</v>
       </c>
@@ -14082,7 +14090,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="136" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:19" ht="20.399999999999999">
       <c r="A136" s="2">
         <v>110</v>
       </c>
@@ -14128,7 +14136,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="137" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:19" ht="20.399999999999999">
       <c r="A137" s="2">
         <v>115</v>
       </c>
@@ -14169,14 +14177,14 @@
       <c r="N137">
         <v>-83.430554000000001</v>
       </c>
-      <c r="O137" s="42" t="s">
+      <c r="O137" s="38" t="s">
         <v>816</v>
       </c>
-      <c r="P137" s="47" t="s">
+      <c r="P137" s="43" t="s">
         <v>819</v>
       </c>
     </row>
-    <row r="138" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:19" ht="20.399999999999999">
       <c r="A138" s="9">
         <v>116</v>
       </c>
@@ -14218,11 +14226,11 @@
         <v>-83.430554000000001</v>
       </c>
       <c r="O138" s="10"/>
-      <c r="P138" s="47" t="s">
+      <c r="P138" s="43" t="s">
         <v>820</v>
       </c>
     </row>
-    <row r="139" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:19" ht="20.399999999999999">
       <c r="A139" s="2">
         <v>107</v>
       </c>
@@ -14263,11 +14271,11 @@
       <c r="N139">
         <v>-83.430554000000001</v>
       </c>
-      <c r="P139" s="47" t="s">
+      <c r="P139" s="43" t="s">
         <v>818</v>
       </c>
     </row>
-    <row r="140" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:19">
       <c r="A140" s="2">
         <v>96</v>
       </c>
@@ -14299,7 +14307,7 @@
         <v>16</v>
       </c>
       <c r="K140" s="2" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="L140" s="2"/>
       <c r="M140">
@@ -14318,7 +14326,7 @@
         <v>1978</v>
       </c>
     </row>
-    <row r="141" spans="1:19" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="141" spans="1:19" ht="21" thickBot="1">
       <c r="A141" s="4">
         <v>263</v>
       </c>
@@ -14370,7 +14378,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="142" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:19" ht="20.399999999999999">
       <c r="A142" s="2">
         <v>261</v>
       </c>
@@ -14420,7 +14428,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="143" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:19" ht="20.399999999999999">
       <c r="A143" s="2">
         <v>143</v>
       </c>
@@ -14456,7 +14464,7 @@
       </c>
       <c r="L143" s="27"/>
     </row>
-    <row r="144" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:19" ht="20.399999999999999">
       <c r="A144" s="2">
         <v>142</v>
       </c>
@@ -14492,7 +14500,7 @@
       </c>
       <c r="L144" s="27"/>
     </row>
-    <row r="145" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:19">
       <c r="A145" s="2">
         <v>186</v>
       </c>
@@ -14528,7 +14536,7 @@
       </c>
       <c r="L145" s="27"/>
     </row>
-    <row r="146" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:19" ht="20.399999999999999">
       <c r="A146" s="2">
         <v>297</v>
       </c>
@@ -14583,7 +14591,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="147" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:19" ht="20.399999999999999">
       <c r="A147" s="2">
         <v>300</v>
       </c>
@@ -14638,7 +14646,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="148" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:19">
       <c r="A148" s="2">
         <v>250</v>
       </c>
@@ -14692,7 +14700,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="149" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:19" ht="20.399999999999999">
       <c r="A149" s="2">
         <v>243</v>
       </c>
@@ -14746,7 +14754,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="150" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:19">
       <c r="A150" s="2">
         <v>236</v>
       </c>
@@ -14800,7 +14808,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="151" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:19">
       <c r="A151" s="2">
         <v>198</v>
       </c>
@@ -14855,7 +14863,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="152" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:19">
       <c r="A152" s="2">
         <v>196</v>
       </c>
@@ -14891,7 +14899,7 @@
       </c>
       <c r="L152" s="27"/>
     </row>
-    <row r="153" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:19">
       <c r="A153" s="2">
         <v>202</v>
       </c>
@@ -14939,7 +14947,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="154" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:19">
       <c r="A154" s="2">
         <v>229</v>
       </c>
@@ -14987,7 +14995,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="155" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:19">
       <c r="A155" s="2">
         <v>262</v>
       </c>
@@ -15035,7 +15043,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="156" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:19">
       <c r="A156" s="2">
         <v>266</v>
       </c>
@@ -15083,38 +15091,38 @@
         <v>577</v>
       </c>
     </row>
-    <row r="157" spans="1:19" ht="20" x14ac:dyDescent="0.35">
-      <c r="A157" s="56">
+    <row r="157" spans="1:19" ht="20.399999999999999">
+      <c r="A157" s="52">
         <v>120</v>
       </c>
-      <c r="B157" s="56" t="s">
+      <c r="B157" s="52" t="s">
         <v>223</v>
       </c>
-      <c r="C157" s="56">
+      <c r="C157" s="52">
         <v>0.68</v>
       </c>
-      <c r="D157" s="56">
+      <c r="D157" s="52">
         <v>1230</v>
       </c>
-      <c r="E157" s="56" t="s">
+      <c r="E157" s="52" t="s">
         <v>24</v>
       </c>
-      <c r="F157" s="56" t="s">
+      <c r="F157" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="G157" s="56">
+      <c r="G157" s="52">
         <v>-30</v>
       </c>
-      <c r="H157" s="56">
+      <c r="H157" s="52">
         <v>19</v>
       </c>
-      <c r="I157" s="56" t="s">
-        <v>15</v>
-      </c>
-      <c r="J157" s="56" t="s">
-        <v>16</v>
-      </c>
-      <c r="K157" s="56" t="s">
+      <c r="I157" s="52" t="s">
+        <v>15</v>
+      </c>
+      <c r="J157" s="52" t="s">
+        <v>16</v>
+      </c>
+      <c r="K157" s="52" t="s">
         <v>224</v>
       </c>
       <c r="L157" s="2" t="s">
@@ -15127,117 +15135,117 @@
         <v>1983</v>
       </c>
     </row>
-    <row r="158" spans="1:19" ht="40" x14ac:dyDescent="0.35">
-      <c r="A158" s="56">
+    <row r="158" spans="1:19" ht="51">
+      <c r="A158" s="52">
         <v>121</v>
       </c>
-      <c r="B158" s="56" t="s">
+      <c r="B158" s="52" t="s">
         <v>225</v>
       </c>
-      <c r="C158" s="56">
+      <c r="C158" s="52">
         <v>0.5</v>
       </c>
-      <c r="D158" s="56">
+      <c r="D158" s="52">
         <v>1230</v>
       </c>
-      <c r="E158" s="56" t="s">
+      <c r="E158" s="52" t="s">
         <v>24</v>
       </c>
-      <c r="F158" s="56" t="s">
+      <c r="F158" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="G158" s="56">
+      <c r="G158" s="52">
         <v>-100</v>
       </c>
-      <c r="H158" s="56">
+      <c r="H158" s="52">
         <v>57.4</v>
       </c>
-      <c r="I158" s="56" t="s">
-        <v>15</v>
-      </c>
-      <c r="J158" s="56" t="s">
-        <v>16</v>
-      </c>
-      <c r="K158" s="56" t="s">
+      <c r="I158" s="52" t="s">
+        <v>15</v>
+      </c>
+      <c r="J158" s="52" t="s">
+        <v>16</v>
+      </c>
+      <c r="K158" s="52" t="s">
         <v>224</v>
       </c>
       <c r="L158" s="2" t="s">
         <v>824</v>
       </c>
     </row>
-    <row r="159" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A159" s="56">
+    <row r="159" spans="1:19">
+      <c r="A159" s="52">
         <v>127</v>
       </c>
-      <c r="B159" s="56" t="s">
+      <c r="B159" s="52" t="s">
         <v>235</v>
       </c>
-      <c r="C159" s="56">
+      <c r="C159" s="52">
         <v>3.03</v>
       </c>
-      <c r="D159" s="56">
+      <c r="D159" s="52">
         <v>2480</v>
       </c>
-      <c r="E159" s="56" t="s">
+      <c r="E159" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="F159" s="56" t="s">
+      <c r="F159" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="G159" s="56">
+      <c r="G159" s="52">
         <v>-25</v>
       </c>
-      <c r="H159" s="56">
+      <c r="H159" s="52">
         <v>7.9</v>
       </c>
-      <c r="I159" s="56" t="s">
-        <v>15</v>
-      </c>
-      <c r="J159" s="56" t="s">
-        <v>16</v>
-      </c>
-      <c r="K159" s="56" t="s">
+      <c r="I159" s="52" t="s">
+        <v>15</v>
+      </c>
+      <c r="J159" s="52" t="s">
+        <v>16</v>
+      </c>
+      <c r="K159" s="52" t="s">
         <v>236</v>
       </c>
       <c r="L159" s="2"/>
     </row>
-    <row r="160" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A160" s="56">
+    <row r="160" spans="1:19">
+      <c r="A160" s="52">
         <v>301</v>
       </c>
-      <c r="B160" s="56" t="s">
+      <c r="B160" s="52" t="s">
         <v>504</v>
       </c>
-      <c r="C160" s="56">
+      <c r="C160" s="52">
         <v>0.6</v>
       </c>
-      <c r="D160" s="56">
+      <c r="D160" s="52">
         <v>749</v>
       </c>
-      <c r="E160" s="56" t="s">
+      <c r="E160" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="F160" s="56" t="s">
-        <v>14</v>
-      </c>
-      <c r="G160" s="56">
+      <c r="F160" s="52" t="s">
+        <v>14</v>
+      </c>
+      <c r="G160" s="52">
         <v>-62</v>
       </c>
-      <c r="H160" s="56">
+      <c r="H160" s="52">
         <v>18.8</v>
       </c>
-      <c r="I160" s="56" t="s">
-        <v>15</v>
-      </c>
-      <c r="J160" s="56" t="s">
-        <v>16</v>
-      </c>
-      <c r="K160" s="56" t="s">
+      <c r="I160" s="52" t="s">
+        <v>15</v>
+      </c>
+      <c r="J160" s="52" t="s">
+        <v>16</v>
+      </c>
+      <c r="K160" s="52" t="s">
         <v>505</v>
       </c>
       <c r="L160" s="2"/>
     </row>
-    <row r="161" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:19">
       <c r="A161" s="2">
         <v>183</v>
       </c>
@@ -15291,7 +15299,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="162" spans="1:19" ht="60" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:19" ht="71.400000000000006">
       <c r="A162" s="2">
         <v>185</v>
       </c>
@@ -15330,11 +15338,11 @@
       <c r="N162" s="10"/>
       <c r="O162" s="10"/>
       <c r="P162" s="27" t="s">
-        <v>827</v>
+        <v>841</v>
       </c>
       <c r="Q162" s="10"/>
     </row>
-    <row r="163" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:19" ht="20.399999999999999">
       <c r="A163" s="2">
         <v>93</v>
       </c>
@@ -15388,7 +15396,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="164" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:19">
       <c r="A164" s="2">
         <v>193</v>
       </c>
@@ -15443,7 +15451,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="165" spans="1:19" ht="30" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:19" ht="30.6">
       <c r="A165" s="2">
         <v>78</v>
       </c>
@@ -15487,8 +15495,8 @@
       <c r="O165">
         <v>4</v>
       </c>
-      <c r="P165" s="47" t="s">
-        <v>831</v>
+      <c r="P165" s="43" t="s">
+        <v>830</v>
       </c>
       <c r="Q165">
         <v>1971</v>
@@ -15500,7 +15508,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="166" spans="1:19" ht="30" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:19" ht="30.6">
       <c r="A166" s="2">
         <v>79</v>
       </c>
@@ -15544,8 +15552,8 @@
       <c r="O166">
         <v>7</v>
       </c>
-      <c r="P166" s="47" t="s">
-        <v>830</v>
+      <c r="P166" s="43" t="s">
+        <v>829</v>
       </c>
       <c r="Q166">
         <v>1970</v>
@@ -15557,7 +15565,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="167" spans="1:19" ht="30" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:19" ht="30.6">
       <c r="A167" s="2">
         <v>213</v>
       </c>
@@ -15611,7 +15619,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="168" spans="1:19" ht="30" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:19" ht="30.6">
       <c r="A168" s="2">
         <v>214</v>
       </c>
@@ -15665,7 +15673,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="169" spans="1:19" ht="30.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="169" spans="1:19" ht="31.2" thickBot="1">
       <c r="A169" s="4">
         <v>215</v>
       </c>
@@ -15719,7 +15727,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="170" spans="1:19" ht="30" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:19" ht="30.6">
       <c r="A170" s="2">
         <v>219</v>
       </c>
@@ -15765,7 +15773,7 @@
         <v>12</v>
       </c>
       <c r="P170" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="Q170">
         <v>1972</v>
@@ -15777,7 +15785,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="171" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:19" ht="20.399999999999999">
       <c r="A171" s="2">
         <v>139</v>
       </c>
@@ -15822,7 +15830,7 @@
         <v>5</v>
       </c>
       <c r="P171" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="Q171">
         <v>1964</v>
@@ -15834,7 +15842,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="172" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:19">
       <c r="A172" s="2">
         <v>137</v>
       </c>
@@ -15889,7 +15897,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="173" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:19">
       <c r="A173" s="9">
         <v>144</v>
       </c>
@@ -15927,7 +15935,7 @@
       <c r="M173" s="10"/>
       <c r="N173" s="10"/>
     </row>
-    <row r="174" spans="1:19" ht="30" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:19" ht="30.6">
       <c r="A174" s="2">
         <v>134</v>
       </c>
@@ -15969,10 +15977,10 @@
         <v>-79.670000999999999</v>
       </c>
       <c r="P174" t="s">
-        <v>833</v>
-      </c>
-    </row>
-    <row r="175" spans="1:19" x14ac:dyDescent="0.35">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="175" spans="1:19">
       <c r="A175" s="2">
         <v>207</v>
       </c>
@@ -16010,7 +16018,7 @@
       <c r="M175" s="10"/>
       <c r="N175" s="10"/>
     </row>
-    <row r="176" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:19">
       <c r="A176" s="2">
         <v>208</v>
       </c>
@@ -16048,7 +16056,7 @@
       <c r="M176" s="10"/>
       <c r="N176" s="10"/>
     </row>
-    <row r="177" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:19">
       <c r="A177" s="2">
         <v>187</v>
       </c>
@@ -16093,7 +16101,7 @@
         <v>2</v>
       </c>
       <c r="P177" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="Q177">
         <v>1959</v>
@@ -16102,7 +16110,7 @@
         <v>1960</v>
       </c>
     </row>
-    <row r="178" spans="1:19" ht="30" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:19" ht="30.6">
       <c r="A178" s="2">
         <v>133</v>
       </c>
@@ -16153,7 +16161,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="179" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:19">
       <c r="A179" s="2">
         <v>135</v>
       </c>
@@ -16204,7 +16212,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="180" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:19">
       <c r="A180" s="2">
         <v>136</v>
       </c>
@@ -16255,7 +16263,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="181" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:19">
       <c r="A181" s="2">
         <v>138</v>
       </c>
@@ -16306,7 +16314,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="182" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:19">
       <c r="A182" s="2">
         <v>140</v>
       </c>
@@ -16357,7 +16365,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="183" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:19">
       <c r="A183" s="2">
         <v>141</v>
       </c>
@@ -16408,7 +16416,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="184" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:19">
       <c r="A184" s="2">
         <v>145</v>
       </c>
@@ -16446,10 +16454,10 @@
       <c r="M184" s="10"/>
       <c r="N184" s="10"/>
       <c r="P184" t="s">
-        <v>835</v>
-      </c>
-    </row>
-    <row r="185" spans="1:19" x14ac:dyDescent="0.35">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="185" spans="1:19">
       <c r="A185" s="2">
         <v>146</v>
       </c>
@@ -16487,10 +16495,10 @@
       <c r="M185" s="10"/>
       <c r="N185" s="10"/>
       <c r="P185" t="s">
-        <v>836</v>
-      </c>
-    </row>
-    <row r="186" spans="1:19" x14ac:dyDescent="0.35">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="186" spans="1:19">
       <c r="A186" s="2">
         <v>147</v>
       </c>
@@ -16528,10 +16536,10 @@
       <c r="M186" s="10"/>
       <c r="N186" s="10"/>
       <c r="P186" t="s">
-        <v>837</v>
-      </c>
-    </row>
-    <row r="187" spans="1:19" x14ac:dyDescent="0.35">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="187" spans="1:19">
       <c r="A187" s="2">
         <v>148</v>
       </c>
@@ -16569,10 +16577,10 @@
       <c r="M187" s="10"/>
       <c r="N187" s="10"/>
       <c r="P187" t="s">
-        <v>838</v>
-      </c>
-    </row>
-    <row r="188" spans="1:19" x14ac:dyDescent="0.35">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="188" spans="1:19">
       <c r="A188" s="2">
         <v>149</v>
       </c>
@@ -16610,10 +16618,10 @@
       <c r="M188" s="10"/>
       <c r="N188" s="10"/>
       <c r="P188" t="s">
-        <v>839</v>
-      </c>
-    </row>
-    <row r="189" spans="1:19" x14ac:dyDescent="0.35">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="189" spans="1:19" ht="20.399999999999999">
       <c r="A189" s="2">
         <v>306</v>
       </c>
@@ -16664,7 +16672,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="190" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:19" ht="20.399999999999999">
       <c r="A190" s="2">
         <v>92</v>
       </c>
@@ -16712,7 +16720,7 @@
         <v>1972</v>
       </c>
     </row>
-    <row r="191" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:19">
       <c r="A191" s="2">
         <v>101</v>
       </c>
@@ -16758,7 +16766,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="192" spans="1:19" ht="20" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:19" ht="20.399999999999999">
       <c r="A192" s="2">
         <v>166</v>
       </c>
@@ -16800,7 +16808,7 @@
         <v>-3.725406</v>
       </c>
       <c r="P192" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="Q192">
         <v>1983</v>
@@ -16809,7 +16817,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="193" spans="1:20" ht="20" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:20" ht="20.399999999999999">
       <c r="A193" s="2">
         <v>177</v>
       </c>
@@ -16851,7 +16859,7 @@
         <v>-3.725406</v>
       </c>
       <c r="P193" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="Q193">
         <v>1983</v>
@@ -16860,7 +16868,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="194" spans="1:20" ht="20" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:20" ht="20.399999999999999">
       <c r="A194" s="2">
         <v>258</v>
       </c>
@@ -16905,7 +16913,7 @@
         <v>17</v>
       </c>
       <c r="P194" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="Q194">
         <v>1983</v>
@@ -16917,7 +16925,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="195" spans="1:20" ht="20" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:20" ht="20.399999999999999">
       <c r="A195" s="2">
         <v>272</v>
       </c>
@@ -16962,7 +16970,7 @@
         <v>17</v>
       </c>
       <c r="P195" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="Q195">
         <v>1983</v>
@@ -16974,7 +16982,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="196" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:20">
       <c r="A196" s="2">
         <v>86</v>
       </c>
@@ -17017,7 +17025,7 @@
       <c r="R196" s="12"/>
       <c r="S196" s="12"/>
     </row>
-    <row r="197" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="197" spans="1:20" ht="15" thickBot="1">
       <c r="A197" s="4">
         <v>87</v>
       </c>
@@ -17060,7 +17068,7 @@
       <c r="R197" s="12"/>
       <c r="S197" s="12"/>
     </row>
-    <row r="198" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:20">
       <c r="A198" s="2">
         <v>206</v>
       </c>
@@ -17103,7 +17111,7 @@
       <c r="R198" s="12"/>
       <c r="S198" s="12"/>
     </row>
-    <row r="199" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:20">
       <c r="A199" s="2">
         <v>232</v>
       </c>
@@ -17146,7 +17154,7 @@
       <c r="R199" s="12"/>
       <c r="S199" s="12"/>
     </row>
-    <row r="200" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:20">
       <c r="A200" s="2">
         <v>238</v>
       </c>
@@ -17189,7 +17197,7 @@
       <c r="R200" s="12"/>
       <c r="S200" s="12"/>
     </row>
-    <row r="201" spans="1:20" ht="20" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:20" ht="20.399999999999999">
       <c r="A201" s="2">
         <v>67</v>
       </c>
@@ -17239,7 +17247,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="202" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:20">
       <c r="A202" s="2">
         <v>167</v>
       </c>
@@ -17286,7 +17294,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="203" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:20">
       <c r="A203" s="9">
         <v>228</v>
       </c>
@@ -17322,7 +17330,7 @@
       </c>
       <c r="L203" s="9"/>
     </row>
-    <row r="204" spans="1:20" ht="20" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:20" ht="20.399999999999999">
       <c r="A204" s="2">
         <v>95</v>
       </c>
@@ -17371,7 +17379,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="205" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:20">
       <c r="A205" s="2">
         <v>269</v>
       </c>
@@ -17420,7 +17428,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="206" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:20">
       <c r="A206" s="2">
         <v>194</v>
       </c>
@@ -17478,7 +17486,7 @@
       </c>
       <c r="T206" s="31"/>
     </row>
-    <row r="207" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:20">
       <c r="A207" s="2">
         <v>85</v>
       </c>
@@ -17534,7 +17542,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="208" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:20">
       <c r="A208" s="9">
         <v>286</v>
       </c>
@@ -17590,7 +17598,7 @@
       </c>
       <c r="T208" s="31"/>
     </row>
-    <row r="209" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:20">
       <c r="A209" s="2">
         <v>299</v>
       </c>
@@ -17644,7 +17652,7 @@
       </c>
       <c r="T209" s="31"/>
     </row>
-    <row r="210" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:20">
       <c r="A210" s="2">
         <v>227</v>
       </c>
@@ -17700,7 +17708,7 @@
       </c>
       <c r="T210" s="31"/>
     </row>
-    <row r="211" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:20">
       <c r="A211" s="2">
         <v>296</v>
       </c>
@@ -17756,7 +17764,7 @@
       </c>
       <c r="T211" s="31"/>
     </row>
-    <row r="212" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:20">
       <c r="A212" s="2">
         <v>302</v>
       </c>
@@ -17807,7 +17815,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="213" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:20">
       <c r="A213" s="2">
         <v>125</v>
       </c>
@@ -17863,7 +17871,7 @@
       </c>
       <c r="T213" s="31"/>
     </row>
-    <row r="214" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:20">
       <c r="A214" s="2">
         <v>118</v>
       </c>
@@ -17921,7 +17929,7 @@
       </c>
       <c r="T214" s="31"/>
     </row>
-    <row r="215" spans="1:20" ht="20" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:20" ht="20.399999999999999">
       <c r="A215" s="2">
         <v>113</v>
       </c>
@@ -17975,7 +17983,7 @@
       </c>
       <c r="T215" s="31"/>
     </row>
-    <row r="216" spans="1:20" ht="20" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:20" ht="30.6">
       <c r="A216" s="2">
         <v>114</v>
       </c>
@@ -18033,7 +18041,7 @@
       </c>
       <c r="T216" s="31"/>
     </row>
-    <row r="217" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:20" ht="20.399999999999999">
       <c r="A217" s="2">
         <v>109</v>
       </c>
@@ -18091,7 +18099,7 @@
       </c>
       <c r="T217" s="31"/>
     </row>
-    <row r="218" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:20" ht="20.399999999999999">
       <c r="A218" s="2">
         <v>106</v>
       </c>
@@ -18149,7 +18157,7 @@
       </c>
       <c r="T218" s="31"/>
     </row>
-    <row r="219" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:20">
       <c r="A219" s="2">
         <v>108</v>
       </c>
@@ -18207,7 +18215,7 @@
       </c>
       <c r="T219" s="31"/>
     </row>
-    <row r="220" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:20">
       <c r="A220" s="2">
         <v>242</v>
       </c>
@@ -18242,7 +18250,7 @@
         <v>417</v>
       </c>
       <c r="L220" s="28"/>
-      <c r="M220" s="49">
+      <c r="M220" s="45">
         <v>35.678013</v>
       </c>
       <c r="N220" s="31">
@@ -18263,7 +18271,7 @@
       </c>
       <c r="T220" s="31"/>
     </row>
-    <row r="221" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:20">
       <c r="A221" s="2">
         <v>294</v>
       </c>
@@ -18298,7 +18306,7 @@
         <v>493</v>
       </c>
       <c r="L221" s="28"/>
-      <c r="M221" s="49">
+      <c r="M221" s="45">
         <v>36.331859000000001</v>
       </c>
       <c r="N221" s="31">
@@ -18319,7 +18327,7 @@
       </c>
       <c r="T221" s="31"/>
     </row>
-    <row r="222" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:20" ht="20.399999999999999">
       <c r="A222" s="2">
         <v>223</v>
       </c>
@@ -18367,7 +18375,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="223" spans="1:20" ht="20" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:20" ht="20.399999999999999">
       <c r="A223" s="2">
         <v>126</v>
       </c>
@@ -18412,7 +18420,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="224" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:20" ht="20.399999999999999">
       <c r="A224" s="2">
         <v>222</v>
       </c>
@@ -18460,7 +18468,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="225" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:20" ht="20.399999999999999">
       <c r="A225" s="2">
         <v>151</v>
       </c>
@@ -18508,7 +18516,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="226" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:20" ht="20.399999999999999">
       <c r="A226" s="2">
         <v>152</v>
       </c>
@@ -18556,7 +18564,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="227" spans="1:20" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="227" spans="1:20" ht="21" thickBot="1">
       <c r="A227" s="4">
         <v>184</v>
       </c>
@@ -18614,7 +18622,7 @@
       </c>
       <c r="T227" s="31"/>
     </row>
-    <row r="228" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:20" ht="20.399999999999999">
       <c r="A228" s="6">
         <v>212</v>
       </c>
@@ -18673,7 +18681,7 @@
       </c>
       <c r="T228" s="31"/>
     </row>
-    <row r="229" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:20">
       <c r="A229" s="2">
         <v>291</v>
       </c>
@@ -18731,7 +18739,7 @@
       </c>
       <c r="T229" s="31"/>
     </row>
-    <row r="230" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:20">
       <c r="A230" s="2">
         <v>201</v>
       </c>
@@ -18789,7 +18797,7 @@
       </c>
       <c r="T230" s="31"/>
     </row>
-    <row r="231" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:20">
       <c r="A231" s="2">
         <v>230</v>
       </c>
@@ -18847,7 +18855,7 @@
       </c>
       <c r="T231" s="31"/>
     </row>
-    <row r="232" spans="1:20" ht="20" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:20" ht="20.399999999999999">
       <c r="A232" s="2">
         <v>248</v>
       </c>
@@ -18894,7 +18902,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="233" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:20">
       <c r="A233" s="2">
         <v>159</v>
       </c>
@@ -18952,7 +18960,7 @@
       </c>
       <c r="T233" s="31"/>
     </row>
-    <row r="234" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:20">
       <c r="A234" s="2">
         <v>160</v>
       </c>
@@ -19010,7 +19018,7 @@
       </c>
       <c r="T234" s="31"/>
     </row>
-    <row r="235" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:20">
       <c r="A235" s="2">
         <v>165</v>
       </c>
@@ -19068,7 +19076,7 @@
       </c>
       <c r="T235" s="31"/>
     </row>
-    <row r="236" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:20">
       <c r="A236" s="2">
         <v>239</v>
       </c>
@@ -19126,7 +19134,7 @@
       </c>
       <c r="T236" s="31"/>
     </row>
-    <row r="237" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:20">
       <c r="A237" s="2">
         <v>240</v>
       </c>
@@ -19184,7 +19192,7 @@
       </c>
       <c r="T237" s="31"/>
     </row>
-    <row r="238" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:20">
       <c r="A238" s="2">
         <v>268</v>
       </c>
@@ -19234,7 +19242,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="239" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:20">
       <c r="A239" s="2">
         <v>99</v>
       </c>
@@ -19288,7 +19296,7 @@
       </c>
       <c r="T239" s="31"/>
     </row>
-    <row r="240" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:20">
       <c r="A240" s="2">
         <v>98</v>
       </c>
@@ -19342,7 +19350,7 @@
       </c>
       <c r="T240" s="31"/>
     </row>
-    <row r="241" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:20">
       <c r="A241" s="2">
         <v>279</v>
       </c>
@@ -19390,7 +19398,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="242" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:20">
       <c r="A242" s="2">
         <v>280</v>
       </c>
@@ -19438,7 +19446,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="243" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:20">
       <c r="A243" s="2">
         <v>298</v>
       </c>
@@ -19488,7 +19496,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="244" spans="1:20" ht="20" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:20" ht="20.399999999999999">
       <c r="A244" s="2">
         <v>281</v>
       </c>
@@ -19535,7 +19543,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="245" spans="1:20" ht="20" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:20" ht="20.399999999999999">
       <c r="A245" s="9">
         <v>282</v>
       </c>
@@ -19582,7 +19590,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="246" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:20">
       <c r="A246" s="2">
         <v>247</v>
       </c>
@@ -19638,7 +19646,7 @@
       <c r="S246" s="31"/>
       <c r="T246" s="31"/>
     </row>
-    <row r="247" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:20">
       <c r="A247" s="2">
         <v>178</v>
       </c>
@@ -19694,7 +19702,7 @@
       </c>
       <c r="T247" s="31"/>
     </row>
-    <row r="248" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:20">
       <c r="A248" s="2">
         <v>203</v>
       </c>
@@ -19752,7 +19760,7 @@
       </c>
       <c r="T248" s="31"/>
     </row>
-    <row r="249" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:20">
       <c r="A249" s="2">
         <v>293</v>
       </c>
@@ -19812,7 +19820,7 @@
       </c>
       <c r="T249" s="31"/>
     </row>
-    <row r="250" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:20">
       <c r="A250" s="2">
         <v>195</v>
       </c>
@@ -19859,7 +19867,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="251" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:20">
       <c r="A251" s="9">
         <v>267</v>
       </c>
@@ -19906,7 +19914,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="252" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:20">
       <c r="A252" s="2">
         <v>311</v>
       </c>
@@ -19957,7 +19965,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="253" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="253" spans="1:20" ht="15" thickBot="1">
       <c r="A253" s="4">
         <v>312</v>
       </c>
@@ -20025,61 +20033,61 @@
       <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="11" max="11" width="14.1796875" customWidth="1"/>
-    <col min="12" max="12" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.21875" customWidth="1"/>
+    <col min="12" max="12" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A1" s="37" t="s">
+    <row r="1" spans="1:17">
+      <c r="A1" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="D1" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="37" t="s">
+      <c r="E1" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="37" t="s">
+      <c r="F1" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="35" t="s">
+      <c r="G1" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="35" t="s">
+      <c r="H1" s="53" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="37" t="s">
+      <c r="J1" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="37" t="s">
+      <c r="K1" s="55" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="38"/>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
+    <row r="2" spans="1:17" ht="15" thickBot="1">
+      <c r="A2" s="56"/>
+      <c r="B2" s="56"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
       <c r="I2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="56"/>
       <c r="L2" t="s">
         <v>519</v>
       </c>
@@ -20096,7 +20104,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17">
       <c r="A3">
         <v>313</v>
       </c>
@@ -20143,7 +20151,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17">
       <c r="A4">
         <v>314</v>
       </c>
@@ -20190,7 +20198,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17">
       <c r="A5">
         <v>315</v>
       </c>
@@ -20237,7 +20245,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17">
       <c r="A6">
         <v>316</v>
       </c>
@@ -20284,7 +20292,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17">
       <c r="A7">
         <v>317</v>
       </c>
@@ -20331,7 +20339,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17">
       <c r="A8">
         <v>318</v>
       </c>
@@ -20378,7 +20386,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17">
       <c r="A9">
         <v>319</v>
       </c>
@@ -20425,7 +20433,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17">
       <c r="A10">
         <v>320</v>
       </c>
@@ -20472,7 +20480,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17">
       <c r="A11">
         <v>321</v>
       </c>
@@ -20519,7 +20527,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17">
       <c r="A12">
         <v>322</v>
       </c>
@@ -20566,7 +20574,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17">
       <c r="A13">
         <v>323</v>
       </c>
@@ -20613,7 +20621,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17">
       <c r="A14">
         <v>324</v>
       </c>
@@ -20666,7 +20674,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17">
       <c r="A15">
         <v>325</v>
       </c>
@@ -20713,7 +20721,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17">
       <c r="A16">
         <v>326</v>
       </c>
@@ -20760,7 +20768,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:19">
       <c r="A17">
         <v>327</v>
       </c>
@@ -20807,7 +20815,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:19" s="10" customFormat="1">
       <c r="A18">
         <v>328</v>
       </c>
@@ -20855,7 +20863,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:19">
       <c r="A19">
         <v>329</v>
       </c>
@@ -20905,7 +20913,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:19">
       <c r="A20">
         <v>330</v>
       </c>
@@ -20955,7 +20963,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:19">
       <c r="A21">
         <v>331</v>
       </c>
@@ -21005,7 +21013,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:19">
       <c r="A22">
         <v>332</v>
       </c>
@@ -21055,7 +21063,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:19">
       <c r="A23">
         <v>333</v>
       </c>
@@ -21102,7 +21110,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:19">
       <c r="A24">
         <v>334</v>
       </c>
@@ -21155,7 +21163,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:19">
       <c r="A25">
         <v>335</v>
       </c>
@@ -21205,7 +21213,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:19">
       <c r="A26">
         <v>336</v>
       </c>
@@ -21256,7 +21264,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="27" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:19" ht="15" thickBot="1">
       <c r="A27">
         <v>337</v>
       </c>
@@ -21305,14 +21313,14 @@
         <v>734</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:19">
       <c r="A28">
         <v>204</v>
       </c>
       <c r="B28" t="s">
         <v>68</v>
       </c>
-      <c r="C28" s="45">
+      <c r="C28" s="41">
         <v>1140</v>
       </c>
       <c r="D28">
@@ -21324,10 +21332,10 @@
       <c r="F28" t="s">
         <v>25</v>
       </c>
-      <c r="G28" s="46">
+      <c r="G28" s="42">
         <v>18.899999999999999</v>
       </c>
-      <c r="H28" s="46">
+      <c r="H28" s="42">
         <v>0</v>
       </c>
       <c r="I28" t="s">
@@ -21339,10 +21347,10 @@
       <c r="K28" t="s">
         <v>62</v>
       </c>
-      <c r="M28" s="45">
+      <c r="M28" s="41">
         <v>49.68</v>
       </c>
-      <c r="N28" s="45">
+      <c r="N28" s="41">
         <v>-83.65</v>
       </c>
       <c r="O28">
@@ -21361,11 +21369,11 @@
         <v>597</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:19">
       <c r="K29" t="s">
         <v>823</v>
       </c>
-      <c r="N29" s="45"/>
+      <c r="N29" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="10">

</xml_diff>